<commit_message>
pushing dynamic ebitda multiple
</commit_message>
<xml_diff>
--- a/models/DCF_SN.xlsx
+++ b/models/DCF_SN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="593" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F65AC8B-90A5-47E3-A127-32E6975F8F1B}"/>
+  <xr:revisionPtr revIDLastSave="624" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA26B62B-7EC1-47A6-ADDB-35A2C4243610}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>FY</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>EV/EBITDA Multiple</t>
+  </si>
+  <si>
+    <t>EBITDA Multiple Approach</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
@@ -480,6 +483,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -652,10 +656,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -975,11 +975,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2E0D3-EC22-43DB-ABCF-85A4F712E8DB}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L14" sqref="L14"/>
+      <selection pane="topRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,10 +988,10 @@
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.109375" customWidth="1"/>
-    <col min="10" max="10" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -1609,6 +1609,14 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
+      <c r="G27" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
@@ -1622,6 +1630,29 @@
         <f>D26/B36</f>
         <v>37.035246567721892</v>
       </c>
+      <c r="G28" s="27">
+        <f>D12</f>
+        <v>35428.875993324378</v>
+      </c>
+      <c r="H28" s="26">
+        <f>I28-0.005</f>
+        <v>3.0402449812245599E-2</v>
+      </c>
+      <c r="I28" s="26">
+        <f>J28-0.005</f>
+        <v>3.54024498122456E-2</v>
+      </c>
+      <c r="J28" s="26">
+        <v>4.0402449812245597E-2</v>
+      </c>
+      <c r="K28" s="26">
+        <f>J28+0.005</f>
+        <v>4.5402449812245595E-2</v>
+      </c>
+      <c r="L28" s="26">
+        <f>K28+0.005</f>
+        <v>5.0402449812245592E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1635,6 +1666,26 @@
         <f>DCF!$M$9</f>
         <v>35.979999999999997</v>
       </c>
+      <c r="G29" s="34">
+        <f>G30-1</f>
+        <v>20.92</v>
+      </c>
+      <c r="H29" s="14">
+        <f t="dataTable" ref="H29:L33" dt2D="1" dtr="1" r1="M4" r2="M13" ca="1"/>
+        <v>34165.715863891761</v>
+      </c>
+      <c r="I29" s="14">
+        <v>33378.766525279636</v>
+      </c>
+      <c r="J29" s="14">
+        <v>32613.998305775287</v>
+      </c>
+      <c r="K29" s="14">
+        <v>31870.680599620049</v>
+      </c>
+      <c r="L29" s="16">
+        <v>31148.110245960645</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
@@ -1656,8 +1707,89 @@
         <f>D30/D29</f>
         <v>2.932869838026389E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="G30" s="34">
+        <f>G31-1</f>
+        <v>21.92</v>
+      </c>
+      <c r="H30" s="14">
+        <v>35640.922027802895</v>
+      </c>
+      <c r="I30" s="23">
+        <v>34818.695895583951</v>
+      </c>
+      <c r="J30" s="25">
+        <v>34019.658350656675</v>
+      </c>
+      <c r="K30" s="18">
+        <v>33243.045378925613</v>
+      </c>
+      <c r="L30" s="16">
+        <v>32488.121671328492</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G31" s="34">
+        <v>22.92</v>
+      </c>
+      <c r="H31" s="14">
+        <v>37116.128191714037</v>
+      </c>
+      <c r="I31" s="24">
+        <v>36258.625265888259</v>
+      </c>
+      <c r="J31" s="13">
+        <v>35425.318395538074</v>
+      </c>
+      <c r="K31" s="19">
+        <v>34615.410158231178</v>
+      </c>
+      <c r="L31" s="16">
+        <v>33828.133096696336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G32" s="34">
+        <f>G31+1</f>
+        <v>23.92</v>
+      </c>
+      <c r="H32" s="14">
+        <v>38591.334355625171</v>
+      </c>
+      <c r="I32" s="21">
+        <v>37698.554636192574</v>
+      </c>
+      <c r="J32" s="22">
+        <v>36830.978440419465</v>
+      </c>
+      <c r="K32" s="20">
+        <v>35987.774937536749</v>
+      </c>
+      <c r="L32" s="16">
+        <v>35168.144522064184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G33" s="34">
+        <f>G32+1</f>
+        <v>24.92</v>
+      </c>
+      <c r="H33" s="15">
+        <v>40066.540519536313</v>
+      </c>
+      <c r="I33" s="15">
+        <v>39138.484006496888</v>
+      </c>
+      <c r="J33" s="15">
+        <v>38236.638485300857</v>
+      </c>
+      <c r="K33" s="15">
+        <v>37360.139716842314</v>
+      </c>
+      <c r="L33" s="17">
+        <v>36508.155947432031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1665,16 +1797,36 @@
         <f>'[1]Income Statement'!$F$24</f>
         <v>873</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="I34" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="H35" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="I35">
+        <f>IF(J34="Bull",I32,IF(J34="Bear",K30,IF(J34="Central",J31,"Error")))</f>
+        <v>35425.318395538074</v>
+      </c>
+      <c r="K35" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35">
+        <f>I35-B37</f>
+        <v>35425.318395538074</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -1682,10 +1834,30 @@
         <f>B34+B35</f>
         <v>876</v>
       </c>
+      <c r="I36" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="28">
+        <f>L35/B36</f>
+        <v>40.439861182121092</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I37" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="28">
+        <f>J36-B29</f>
+        <v>4.4598611821210952</v>
+      </c>
+      <c r="K37" s="11">
+        <f>J37/B29</f>
+        <v>0.12395389611231505</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22" xr:uid="{EAB0D90E-FD11-4473-987B-7DCF4EF16CCE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22 J34" xr:uid="{EAB0D90E-FD11-4473-987B-7DCF4EF16CCE}">
       <formula1>$O$2:$O$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
cleanup + landing page sort out
includes a little SOTP
</commit_message>
<xml_diff>
--- a/models/DCF_SN.xlsx
+++ b/models/DCF_SN.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/CB10F4A09BCEF627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="624" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA26B62B-7EC1-47A6-ADDB-35A2C4243610}"/>
+  <xr:revisionPtr revIDLastSave="893" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15FDC869-F90E-4B72-97D0-1F30F5275BC7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="2" r:id="rId1"/>
+    <sheet name="SOTP" sheetId="3" r:id="rId2"/>
+    <sheet name="rNPV" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
   <si>
     <t>FY</t>
   </si>
@@ -198,6 +200,78 @@
   </si>
   <si>
     <t>EBITDA Multiple Approach</t>
+  </si>
+  <si>
+    <t>Orthopaedics</t>
+  </si>
+  <si>
+    <t>Sports Med and ENT</t>
+  </si>
+  <si>
+    <t>Advanced Wound</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Cost of Revenue</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>OpEx</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>SM&amp;E</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>Net Operating Profit after Tax</t>
+  </si>
+  <si>
+    <t>tranche up debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tranche up equity </t>
+  </si>
+  <si>
+    <t>find fcf</t>
+  </si>
+  <si>
+    <t>discount fcf</t>
+  </si>
+  <si>
+    <t>tv + pv of tv</t>
+  </si>
+  <si>
+    <t>individual Enterprise values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum less net debt for overall </t>
+  </si>
+  <si>
+    <t>three scenario models</t>
+  </si>
+  <si>
+    <t>code these locations into the viewer</t>
+  </si>
+  <si>
+    <t>add note that viewer can't see them differently</t>
+  </si>
+  <si>
+    <t>Debt Portion:</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -208,7 +282,7 @@
     <numFmt numFmtId="164" formatCode="0;\(0\);\-"/>
     <numFmt numFmtId="165" formatCode="[Color10]0.00%;[Red]\(0.00\)%;\-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +348,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -440,14 +521,13 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -484,6 +564,49 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -567,6 +690,57 @@
             <v>1375</v>
           </cell>
         </row>
+        <row r="44">
+          <cell r="G44">
+            <v>2413.6991302341535</v>
+          </cell>
+          <cell r="H44">
+            <v>2527.5242912334529</v>
+          </cell>
+          <cell r="I44">
+            <v>2646.7172162238094</v>
+          </cell>
+          <cell r="J44">
+            <v>2771.5310380803335</v>
+          </cell>
+          <cell r="K44">
+            <v>2902.230826911697</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="G45">
+            <v>1972.7566005307594</v>
+          </cell>
+          <cell r="H45">
+            <v>2133.6450684965343</v>
+          </cell>
+          <cell r="I45">
+            <v>2307.6548202118656</v>
+          </cell>
+          <cell r="J45">
+            <v>2495.8559639909986</v>
+          </cell>
+          <cell r="K45">
+            <v>2699.405880996329</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="G46">
+            <v>1789.1296699937484</v>
+          </cell>
+          <cell r="H46">
+            <v>1904.2147388768226</v>
+          </cell>
+          <cell r="I46">
+            <v>2026.7026099725886</v>
+          </cell>
+          <cell r="J46">
+            <v>2157.0694656488554</v>
+          </cell>
+          <cell r="K46">
+            <v>2295.8221185186958</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="3">
@@ -656,6 +830,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -977,9 +1155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2E0D3-EC22-43DB-ABCF-85A4F712E8DB}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M31" sqref="M31"/>
+      <selection pane="topRight" activeCell="A34" sqref="A34:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,10 +1167,10 @@
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1017,7 +1195,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1">
@@ -1040,10 +1218,10 @@
         <f>'[1]Income Statement'!K8</f>
         <v>1107.2169098036211</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="H2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="9">
+      <c r="I2" s="8">
         <f>'[1]Balance Sheet'!$N$7</f>
         <v>0.10567499999999999</v>
       </c>
@@ -1052,33 +1230,33 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5">
-        <f>B2*(1-DCF!$M$2)</f>
+        <f>B2*(1-DCF!$I$2)</f>
         <v>774.31708613862099</v>
       </c>
       <c r="C3" s="5">
-        <f>C2*(1-DCF!$M$2)</f>
+        <f>C2*(1-DCF!$I$2)</f>
         <v>823.19144740343734</v>
       </c>
       <c r="D3" s="5">
-        <f>D2*(1-DCF!$M$2)</f>
+        <f>D2*(1-DCF!$I$2)</f>
         <v>875.31222184361388</v>
       </c>
       <c r="E3" s="5">
-        <f>E2*(1-DCF!$M$2)</f>
+        <f>E2*(1-DCF!$I$2)</f>
         <v>930.90502764999314</v>
       </c>
       <c r="F3" s="5">
-        <f>F2*(1-DCF!$M$2)</f>
+        <f>F2*(1-DCF!$I$2)</f>
         <v>990.21176286012349</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="H3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="9">
+      <c r="I3" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="O3" t="s">
@@ -1086,7 +1264,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
@@ -1109,11 +1287,11 @@
         <f>'[1]Income Statement'!K39</f>
         <v>606.29501506130021</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="H4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="9">
-        <f>(M5*(1-M2)*(M6/(M6+M8)))+(M7*(M7/(M7+M5)))</f>
+      <c r="I4" s="8">
+        <f>(I5*(1-I2)*(I6/(I6+I8)))+(I7*(I7/(I7+I5)))</f>
         <v>4.0402449812245597E-2</v>
       </c>
       <c r="O4" t="s">
@@ -1121,7 +1299,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
@@ -1144,16 +1322,16 @@
         <f>'[1]Balance Sheet'!K53</f>
         <v>-610.64026286698993</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="H5" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="9">
+      <c r="I5" s="8">
         <f>0.056</f>
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="28" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
@@ -1176,126 +1354,128 @@
         <f>-'[1]Balance Sheet'!$G$52</f>
         <v>-149.35645811619816</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="H6" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="2">
+      <c r="I6" s="2">
         <f>'[1]Balance Sheet'!$F$49</f>
         <v>2986</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>SUM(B3:B6)</f>
         <v>621.56276935658195</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f t="shared" ref="C7:F7" si="0">SUM(C3:C6)</f>
         <v>670.22266012225271</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>722.11471815119137</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>777.46357157637021</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>836.51005693823561</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="H7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="9">
-        <f>M3+(M10*M11)</f>
+      <c r="I7" s="8">
+        <f>I3+(I10*I11)</f>
         <v>6.6460000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1">
-        <f>B7/((1+DCF!$M$4)^(DCF!B1-2024))</f>
+        <f>B7/((1+DCF!$I$4)^(DCF!B1-2024))</f>
         <v>597.42532273809161</v>
       </c>
       <c r="C8" s="1">
-        <f>C7/((1+DCF!$M$4)^(DCF!C1-2024))</f>
+        <f>C7/((1+DCF!$I$4)^(DCF!C1-2024))</f>
         <v>619.17922302818999</v>
       </c>
       <c r="D8" s="1">
-        <f>D7/((1+DCF!$M$4)^(DCF!D1-2024))</f>
+        <f>D7/((1+DCF!$I$4)^(DCF!D1-2024))</f>
         <v>641.21267480518929</v>
       </c>
       <c r="E8" s="1">
-        <f>E7/((1+DCF!$M$4)^(DCF!E1-2024))</f>
+        <f>E7/((1+DCF!$I$4)^(DCF!E1-2024))</f>
         <v>663.55142245628178</v>
       </c>
       <c r="F8" s="1">
-        <f>F7/((1+DCF!$M$4)^(DCF!F1-2024))</f>
+        <f>F7/((1+DCF!$I$4)^(DCF!F1-2024))</f>
         <v>686.22152382874856</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="H8" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="8">
-        <f>M9*'[1]Income Statement'!$H$25</f>
+      <c r="I8" s="7">
+        <f>I9*'[1]Income Statement'!$H$25</f>
         <v>31518.479999999996</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="L9" s="2" t="s">
+      <c r="H9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="2">
+      <c r="I9" s="2">
         <v>35.979999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="H10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="M10" s="2">
+      <c r="I10" s="2">
         <v>0.67</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="5">
-        <f>((F7*(1+DCF!M12))/(DCF!M4-DCF!M12))/((1+M4)^5)</f>
+        <f>((F7*(1+DCF!I12))/(DCF!I4-DCF!I12))/((1+I4)^5)</f>
         <v>34306.956309002388</v>
       </c>
       <c r="D11" s="5">
-        <f>((F2+F4)*M13)/((1+M4)^5)</f>
+        <f>((F2+F4)*I13)/((1+I4)^5)</f>
         <v>32221.28582646788</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="H11" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="9">
+      <c r="I11" s="8">
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="47" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="5">
@@ -1306,228 +1486,228 @@
         <f>SUM(B8:F8)+D11</f>
         <v>35428.875993324378</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="H12" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="9">
+      <c r="I12" s="8">
         <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="5"/>
-      <c r="L13" s="2" t="s">
+      <c r="H13" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="32">
-        <f>M8/'[1]Income Statement'!$F$41</f>
+      <c r="I13" s="31">
+        <f>I8/'[1]Income Statement'!$F$41</f>
         <v>22.922530909090906</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1">
         <f>'[1]Balance Sheet'!$F$22</f>
         <v>2</v>
       </c>
-      <c r="G15" s="33" t="s">
+      <c r="G15" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1">
         <f>'[1]Balance Sheet'!$F$28</f>
         <v>3123</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="26">
         <f>B12</f>
         <v>37514.546475858886</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="25">
         <f>I16-0.005</f>
         <v>3.0402449812245599E-2</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="25">
         <f>J16-0.005</f>
         <v>3.54024498122456E-2</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="25">
         <v>4.0402449812245597E-2</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="25">
         <f>J16+0.005</f>
         <v>4.5402449812245595E-2</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="25">
         <f>K16+0.005</f>
         <v>5.0402449812245592E-2</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1">
         <f>'[1]Balance Sheet'!$F$23</f>
         <v>0</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="25">
         <f>G18-0.005</f>
         <v>9.9999999999999985E-3</v>
       </c>
-      <c r="H17" s="14">
-        <f t="dataTable" ref="H17:L21" dt2D="1" dtr="1" r1="M4" r2="M12"/>
+      <c r="H17" s="13">
+        <f t="dataTable" ref="H17:L21" dt2D="1" dtr="1" r1="I4" r2="I12" ca="1"/>
         <v>38955.738924016259</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>31204.748093147573</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <v>26004.560257992824</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="13">
         <v>22274.37262742137</v>
       </c>
-      <c r="L17" s="16">
+      <c r="L17" s="15">
         <v>19468.401621756842</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="28" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="1">
         <f>'[1]Balance Sheet'!$F$24</f>
         <v>61</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="25">
         <f>G19-0.005</f>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <v>50762.792125788292</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="22">
         <v>38226.516443891356</v>
       </c>
-      <c r="J18" s="25">
+      <c r="J18" s="24">
         <v>30626.789961925686</v>
       </c>
-      <c r="K18" s="18">
+      <c r="K18" s="17">
         <v>25527.980580474767</v>
       </c>
-      <c r="L18" s="16">
+      <c r="L18" s="15">
         <v>21870.42512103431</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1">
         <f>'[1]Balance Sheet'!$F$30</f>
         <v>79</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="25">
         <v>0.02</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <v>73920.107443579327</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="23">
         <v>49807.149414444641</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="12">
         <v>37514.546475858886</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="18">
         <v>30062.413011915662</v>
       </c>
-      <c r="L19" s="16">
+      <c r="L19" s="15">
         <v>25062.524260305097</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="28" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="1">
         <f>'[1]Balance Sheet'!$F$29</f>
         <v>135</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="25">
         <f>G19+0.005</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <v>139941.89373766878</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="20">
         <v>72520.384012088427</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="21">
         <v>48874.160777283214</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="19">
         <v>36819.339542432499</v>
       </c>
-      <c r="L20" s="16">
+      <c r="L20" s="15">
         <v>29511.234144942646</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="1">
         <f>'[1]Balance Sheet'!$F$31</f>
         <v>31</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="25">
         <f>G20+0.005</f>
         <v>3.0000000000000002E-2</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>1846461.0609523756</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="14">
         <v>137276.09079736884</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="14">
         <v>71153.908803411527</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="14">
         <v>47963.182838063418</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="16">
         <v>36140.422318009769</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="1">
         <f>'[1]Balance Sheet'!$F$32</f>
         <v>190</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="I22" s="28" t="s">
         <v>25</v>
       </c>
       <c r="J22" s="3" t="s">
@@ -1535,21 +1715,21 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="1">
         <f>'[1]Balance Sheet'!$F$3</f>
         <v>619</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I23">
         <f>IF(J22="Bull",I20,IF(J22="Bear",K18,IF(J22="Central",J19,"Error")))</f>
         <v>37514.546475858886</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="28" t="s">
         <v>40</v>
       </c>
       <c r="L23">
@@ -1558,43 +1738,43 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="1">
         <f>'[1]Balance Sheet'!$F$12</f>
         <v>16</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="I24" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="27">
         <f>L23/B36</f>
         <v>39.416148945044391</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="47" t="s">
         <v>26</v>
       </c>
       <c r="B25">
         <f>SUM(B15:B22)+(-1*SUM(B23:B24))</f>
         <v>2986</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="I25" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="27">
         <f>J24-B29</f>
         <v>3.4361489450443941</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="10">
         <f>J25/B29</f>
         <v>9.5501638272495679E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="47" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="5">
@@ -1607,197 +1787,197 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+      <c r="A27" s="47"/>
       <c r="B27" s="5"/>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <f>B26/B36</f>
         <v>39.416148945044391</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="9">
         <f>D26/B36</f>
         <v>37.035246567721892</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="26">
         <f>D12</f>
         <v>35428.875993324378</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="25">
         <f>I28-0.005</f>
         <v>3.0402449812245599E-2</v>
       </c>
-      <c r="I28" s="26">
+      <c r="I28" s="25">
         <f>J28-0.005</f>
         <v>3.54024498122456E-2</v>
       </c>
-      <c r="J28" s="26">
+      <c r="J28" s="25">
         <v>4.0402449812245597E-2</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="25">
         <f>J28+0.005</f>
         <v>4.5402449812245595E-2</v>
       </c>
-      <c r="L28" s="26">
+      <c r="L28" s="25">
         <f>K28+0.005</f>
         <v>5.0402449812245592E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="28" t="s">
         <v>22</v>
       </c>
       <c r="B29">
-        <f>DCF!$M$9</f>
+        <f>DCF!$I$9</f>
         <v>35.979999999999997</v>
       </c>
       <c r="D29">
-        <f>DCF!$M$9</f>
+        <f>DCF!$I$9</f>
         <v>35.979999999999997</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="33">
         <f>G30-1</f>
         <v>20.92</v>
       </c>
-      <c r="H29" s="14">
-        <f t="dataTable" ref="H29:L33" dt2D="1" dtr="1" r1="M4" r2="M13" ca="1"/>
+      <c r="H29" s="13">
+        <f t="dataTable" ref="H29:L33" dt2D="1" dtr="1" r1="I4" r2="I13"/>
         <v>34165.715863891761</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="13">
         <v>33378.766525279636</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="13">
         <v>32613.998305775287</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="13">
         <v>31870.680599620049</v>
       </c>
-      <c r="L29" s="16">
+      <c r="L29" s="15">
         <v>31148.110245960645</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <f>B28-B29</f>
         <v>3.4361489450443941</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <f>B30/B29</f>
         <v>9.5501638272495679E-2</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="9">
         <f>D28-D29</f>
         <v>1.0552465677218947</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="10">
         <f>D30/D29</f>
         <v>2.932869838026389E-2</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="33">
         <f>G31-1</f>
         <v>21.92</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H30" s="13">
         <v>35640.922027802895</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="22">
         <v>34818.695895583951</v>
       </c>
-      <c r="J30" s="25">
+      <c r="J30" s="24">
         <v>34019.658350656675</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="17">
         <v>33243.045378925613</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="15">
         <v>32488.121671328492</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G31" s="34">
+      <c r="G31" s="33">
         <v>22.92</v>
       </c>
-      <c r="H31" s="14">
+      <c r="H31" s="13">
         <v>37116.128191714037</v>
       </c>
-      <c r="I31" s="24">
+      <c r="I31" s="23">
         <v>36258.625265888259</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="12">
         <v>35425.318395538074</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="18">
         <v>34615.410158231178</v>
       </c>
-      <c r="L31" s="16">
+      <c r="L31" s="15">
         <v>33828.133096696336</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G32" s="34">
+      <c r="G32" s="33">
         <f>G31+1</f>
         <v>23.92</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="13">
         <v>38591.334355625171</v>
       </c>
-      <c r="I32" s="21">
+      <c r="I32" s="20">
         <v>37698.554636192574</v>
       </c>
-      <c r="J32" s="22">
+      <c r="J32" s="21">
         <v>36830.978440419465</v>
       </c>
-      <c r="K32" s="20">
+      <c r="K32" s="19">
         <v>35987.774937536749</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L32" s="15">
         <v>35168.144522064184</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="G33" s="34">
+      <c r="G33" s="33">
         <f>G32+1</f>
         <v>24.92</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>40066.540519536313</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="14">
         <v>39138.484006496888</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="14">
         <v>38236.638485300857</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="14">
         <v>37360.139716842314</v>
       </c>
-      <c r="L33" s="17">
+      <c r="L33" s="16">
         <v>36508.155947432031</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="28" t="s">
         <v>42</v>
       </c>
       <c r="B34">
         <f>'[1]Income Statement'!$F$24</f>
         <v>873</v>
       </c>
-      <c r="I34" s="29" t="s">
+      <c r="I34" s="28" t="s">
         <v>25</v>
       </c>
       <c r="J34" s="3" t="s">
@@ -1805,20 +1985,20 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="28" t="s">
         <v>43</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
-      <c r="H35" s="29" t="s">
+      <c r="H35" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I35">
         <f>IF(J34="Bull",I32,IF(J34="Bear",K30,IF(J34="Central",J31,"Error")))</f>
         <v>35425.318395538074</v>
       </c>
-      <c r="K35" s="29" t="s">
+      <c r="K35" s="28" t="s">
         <v>40</v>
       </c>
       <c r="L35">
@@ -1827,36 +2007,36 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="3">
         <f>B34+B35</f>
         <v>876</v>
       </c>
-      <c r="I36" s="29" t="s">
+      <c r="I36" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36" s="27">
         <f>L35/B36</f>
         <v>40.439861182121092</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I37" s="29" t="s">
+      <c r="I37" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J37" s="28">
+      <c r="J37" s="27">
         <f>J36-B29</f>
         <v>4.4598611821210952</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K37" s="10">
         <f>J37/B29</f>
         <v>0.12395389611231505</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J22 J34" xr:uid="{EAB0D90E-FD11-4473-987B-7DCF4EF16CCE}">
       <formula1>$O$2:$O$4</formula1>
     </dataValidation>
@@ -1866,4 +2046,1110 @@
     <ignoredError sqref="C30:D30" formula="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1EAA58-ADB1-46F6-8416-C90E04EF858D}">
+  <dimension ref="A1:Z26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.21875" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="37"/>
+    <col min="11" max="11" width="8.88671875" style="37"/>
+    <col min="16" max="16" width="8.88671875" style="37"/>
+    <col min="23" max="23" width="37.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" s="35"/>
+      <c r="B1" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="X1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38">
+        <v>2025</v>
+      </c>
+      <c r="C2" s="38">
+        <v>2026</v>
+      </c>
+      <c r="D2" s="38">
+        <v>2027</v>
+      </c>
+      <c r="E2" s="38">
+        <v>2028</v>
+      </c>
+      <c r="F2" s="39">
+        <v>2029</v>
+      </c>
+      <c r="G2" s="38">
+        <v>2025</v>
+      </c>
+      <c r="H2" s="38">
+        <v>2026</v>
+      </c>
+      <c r="I2" s="38">
+        <v>2027</v>
+      </c>
+      <c r="J2" s="38">
+        <v>2028</v>
+      </c>
+      <c r="K2" s="39">
+        <v>2029</v>
+      </c>
+      <c r="L2" s="38">
+        <v>2025</v>
+      </c>
+      <c r="M2" s="38">
+        <v>2026</v>
+      </c>
+      <c r="N2" s="38">
+        <v>2027</v>
+      </c>
+      <c r="O2" s="38">
+        <v>2028</v>
+      </c>
+      <c r="P2" s="39">
+        <v>2029</v>
+      </c>
+      <c r="Q2" s="43">
+        <v>2025</v>
+      </c>
+      <c r="R2" s="43">
+        <v>2026</v>
+      </c>
+      <c r="S2" s="43">
+        <v>2027</v>
+      </c>
+      <c r="T2" s="43">
+        <v>2028</v>
+      </c>
+      <c r="U2" s="43">
+        <v>2029</v>
+      </c>
+      <c r="W2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="8">
+        <f>'[1]Balance Sheet'!$N$7</f>
+        <v>0.10567499999999999</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>'[1]Balance Sheet'!$N$7</f>
+        <v>0.10567499999999999</v>
+      </c>
+      <c r="Z2" s="8">
+        <f>'[1]Balance Sheet'!$N$7</f>
+        <v>0.10567499999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1">
+        <f>'[1]Income Statement'!G44</f>
+        <v>2413.6991302341535</v>
+      </c>
+      <c r="C3" s="1">
+        <f>'[1]Income Statement'!H44</f>
+        <v>2527.5242912334529</v>
+      </c>
+      <c r="D3" s="1">
+        <f>'[1]Income Statement'!I44</f>
+        <v>2646.7172162238094</v>
+      </c>
+      <c r="E3" s="1">
+        <f>'[1]Income Statement'!J44</f>
+        <v>2771.5310380803335</v>
+      </c>
+      <c r="F3" s="40">
+        <f>'[1]Income Statement'!K44</f>
+        <v>2902.230826911697</v>
+      </c>
+      <c r="G3" s="1">
+        <f>'[1]Income Statement'!G45</f>
+        <v>1972.7566005307594</v>
+      </c>
+      <c r="H3" s="1">
+        <f>'[1]Income Statement'!H45</f>
+        <v>2133.6450684965343</v>
+      </c>
+      <c r="I3" s="1">
+        <f>'[1]Income Statement'!I45</f>
+        <v>2307.6548202118656</v>
+      </c>
+      <c r="J3" s="1">
+        <f>'[1]Income Statement'!J45</f>
+        <v>2495.8559639909986</v>
+      </c>
+      <c r="K3" s="40">
+        <f>'[1]Income Statement'!K45</f>
+        <v>2699.405880996329</v>
+      </c>
+      <c r="L3" s="1">
+        <f>'[1]Income Statement'!G46</f>
+        <v>1789.1296699937484</v>
+      </c>
+      <c r="M3" s="1">
+        <f>'[1]Income Statement'!H46</f>
+        <v>1904.2147388768226</v>
+      </c>
+      <c r="N3" s="1">
+        <f>'[1]Income Statement'!I46</f>
+        <v>2026.7026099725886</v>
+      </c>
+      <c r="O3" s="1">
+        <f>'[1]Income Statement'!J46</f>
+        <v>2157.0694656488554</v>
+      </c>
+      <c r="P3" s="46">
+        <f>'[1]Income Statement'!K46</f>
+        <v>2295.8221185186958</v>
+      </c>
+      <c r="Q3" s="44">
+        <v>6175.5854007586613</v>
+      </c>
+      <c r="R3" s="44">
+        <v>6565.3840986068099</v>
+      </c>
+      <c r="S3" s="44">
+        <v>6981.074646408264</v>
+      </c>
+      <c r="T3" s="44">
+        <v>7424.456467720187</v>
+      </c>
+      <c r="U3" s="44">
+        <v>7897.4588264267222</v>
+      </c>
+      <c r="W3" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="8">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1">
+        <f>(B$3/Q$3)*Q4</f>
+        <v>-714.38197475327559</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:F4" si="0">C3/R3*R4</f>
+        <v>-748.07078139563498</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>-783.34828390812493</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>-820.28940196939595</v>
+      </c>
+      <c r="F4" s="40">
+        <f t="shared" si="0"/>
+        <v>-858.97258831836211</v>
+      </c>
+      <c r="G4" s="1">
+        <f>G3/Q3*Q4</f>
+        <v>-583.87631595906737</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:K4" si="1">H3/R3*R4</f>
+        <v>-631.49443870714572</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>-682.99606477959924</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>-738.69791388732926</v>
+      </c>
+      <c r="K4" s="40">
+        <f t="shared" si="1"/>
+        <v>-798.94253586597108</v>
+      </c>
+      <c r="L4" s="1">
+        <f>L3/Q3*Q4</f>
+        <v>-529.52829568937182</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:P4" si="2">M3/R3*R4</f>
+        <v>-563.58999697744082</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="2"/>
+        <v>-599.84270392862948</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="2"/>
+        <v>-638.42735212848697</v>
+      </c>
+      <c r="P4" s="40">
+        <f t="shared" si="2"/>
+        <v>-679.49394278918635</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>-1827.7865864017149</v>
+      </c>
+      <c r="R4" s="44">
+        <v>-1943.1552170802215</v>
+      </c>
+      <c r="S4" s="44">
+        <v>-2066.1870526163539</v>
+      </c>
+      <c r="T4" s="44">
+        <v>-2197.414667985212</v>
+      </c>
+      <c r="U4" s="44">
+        <v>-2337.4090669735197</v>
+      </c>
+      <c r="W4" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="8">
+        <f>(X5*(1-X2)*(X6/(X6+X8)))+(X7*(X7/(X7+X5)))</f>
+        <v>3.6068361914094398E-2</v>
+      </c>
+      <c r="Y4" s="8">
+        <f>(Y5*(1-Y2)*(Y6/(Y6+Y8)))+(Y7*(Y7/(Y7+Y5)))</f>
+        <v>3.6068361914094398E-2</v>
+      </c>
+      <c r="Z4" s="8">
+        <f>(Z5*(1-Z2)*(Z6/(Z6+Z8)))+(Z7*(Z7/(Z7+Z5)))</f>
+        <v>3.6068361914094398E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="5">
+        <f>SUM(B3:B4)</f>
+        <v>1699.3171554808778</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" ref="C5:P5" si="3">SUM(C3:C4)</f>
+        <v>1779.4535098378178</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="3"/>
+        <v>1863.3689323156846</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="3"/>
+        <v>1951.2416361109376</v>
+      </c>
+      <c r="F5" s="41">
+        <f t="shared" si="3"/>
+        <v>2043.2582385933349</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="3"/>
+        <v>1388.8802845716921</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="3"/>
+        <v>1502.1506297893886</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="3"/>
+        <v>1624.6587554322664</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="3"/>
+        <v>1757.1580501036692</v>
+      </c>
+      <c r="K5" s="41">
+        <f t="shared" si="3"/>
+        <v>1900.463345130358</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" si="3"/>
+        <v>1259.6013743043766</v>
+      </c>
+      <c r="M5" s="5">
+        <f t="shared" si="3"/>
+        <v>1340.6247418993817</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="3"/>
+        <v>1426.8599060439592</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" si="3"/>
+        <v>1518.6421135203684</v>
+      </c>
+      <c r="P5" s="41">
+        <f t="shared" si="3"/>
+        <v>1616.3281757295094</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>4347.7988143569464</v>
+      </c>
+      <c r="R5" s="45">
+        <v>4622.2288815265883</v>
+      </c>
+      <c r="S5" s="45">
+        <v>4914.8875937919101</v>
+      </c>
+      <c r="T5" s="45">
+        <v>5227.041799734975</v>
+      </c>
+      <c r="U5" s="45">
+        <v>5560.0497594532026</v>
+      </c>
+      <c r="W5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5" s="8">
+        <f>0.056</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="Y5" s="8">
+        <f>0.056</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="Z5" s="8">
+        <f>0.056</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ref="B6" si="4">B$3/Q$3*Q6</f>
+        <v>-1360.9186211028596</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ref="C6:F6" si="5">C$3/R$3*R6</f>
+        <v>-1425.0967861498636</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="5"/>
+        <v>-1492.3014634400924</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="5"/>
+        <v>-1562.6753771594383</v>
+      </c>
+      <c r="F6" s="40">
+        <f t="shared" si="5"/>
+        <v>-1636.3679820772513</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ref="G6" si="6">G$3/Q$3*Q6</f>
+        <v>-1112.3015122043967</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ref="H6" si="7">H$3/R$3*R6</f>
+        <v>-1203.0154331039303</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6" si="8">I$3/S$3*S6</f>
+        <v>-1301.1275417742045</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6" si="9">J$3/T$3*T6</f>
+        <v>-1407.2411985567014</v>
+      </c>
+      <c r="K6" s="40">
+        <f t="shared" ref="K6" si="10">K$3/U$3*U6</f>
+        <v>-1522.0089709383496</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" ref="L6" si="11">L$3/Q$3*Q6</f>
+        <v>-1008.7669390782356</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6" si="12">M$3/R$3*R6</f>
+        <v>-1073.6554793656437</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6" si="13">N$3/S$3*S6</f>
+        <v>-1142.7179497230422</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" ref="O6" si="14">O$3/T$3*T6</f>
+        <v>-1216.2228365757996</v>
+      </c>
+      <c r="P6" s="40">
+        <f t="shared" ref="P6" si="15">P$3/U$3*U6</f>
+        <v>-1294.45589663398</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>-3481.987072385492</v>
+      </c>
+      <c r="R6" s="44">
+        <v>-3701.7676986194379</v>
+      </c>
+      <c r="S6" s="44">
+        <v>-3936.1469549373396</v>
+      </c>
+      <c r="T6" s="44">
+        <v>-4186.1394122919392</v>
+      </c>
+      <c r="U6" s="44">
+        <v>-4452.8328496495815</v>
+      </c>
+      <c r="W6" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
+        <f>SUM(B5:B6)</f>
+        <v>338.39853437801821</v>
+      </c>
+      <c r="C7" s="5">
+        <f>SUM(C5:C6)</f>
+        <v>354.35672368795417</v>
+      </c>
+      <c r="D7" s="5">
+        <f>SUM(D5:D6)</f>
+        <v>371.06746887559211</v>
+      </c>
+      <c r="E7" s="5">
+        <f>SUM(E5:E6)</f>
+        <v>388.56625895149932</v>
+      </c>
+      <c r="F7" s="41">
+        <f>SUM(F5:F6)</f>
+        <v>406.89025651608358</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" ref="G7:P7" si="16">SUM(G5:G6)</f>
+        <v>276.57877236729541</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="16"/>
+        <v>299.13519668545837</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="16"/>
+        <v>323.53121365806192</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="16"/>
+        <v>349.91685154696779</v>
+      </c>
+      <c r="K7" s="41">
+        <f t="shared" si="16"/>
+        <v>378.45437419200834</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" si="16"/>
+        <v>250.83443522614095</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" si="16"/>
+        <v>266.96926253373795</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="16"/>
+        <v>284.14195632091696</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" si="16"/>
+        <v>302.41927694456876</v>
+      </c>
+      <c r="P7" s="41">
+        <f t="shared" si="16"/>
+        <v>321.87227909552939</v>
+      </c>
+      <c r="Q7" s="45">
+        <v>865.81174197145447</v>
+      </c>
+      <c r="R7" s="45">
+        <v>920.46118290715049</v>
+      </c>
+      <c r="S7" s="45">
+        <v>978.74063885457053</v>
+      </c>
+      <c r="T7" s="45">
+        <v>1040.9023874430359</v>
+      </c>
+      <c r="U7" s="45">
+        <v>1107.2169098036211</v>
+      </c>
+      <c r="W7" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="X7" s="8">
+        <f>X3+(X10*X11)</f>
+        <v>6.6460000000000005E-2</v>
+      </c>
+      <c r="Y7" s="8">
+        <f>Y3+(Y10*Y11)</f>
+        <v>6.6460000000000005E-2</v>
+      </c>
+      <c r="Z7" s="8">
+        <f>Z3+(Z10*Z11)</f>
+        <v>6.6460000000000005E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5">
+        <f>B7*(1-$X$2)</f>
+        <v>302.63826925762118</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" ref="C8:F8" si="17">C7*(1-$X$2)</f>
+        <v>316.91007691222961</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="17"/>
+        <v>331.85491410216395</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="17"/>
+        <v>347.50451953679965</v>
+      </c>
+      <c r="F8" s="41">
+        <f t="shared" si="17"/>
+        <v>363.89212865874646</v>
+      </c>
+      <c r="G8" s="5">
+        <f>G7*(1-$Y$2)</f>
+        <v>247.35131059738148</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ref="H8:K8" si="18">H7*(1-$Y$2)</f>
+        <v>267.52408477572254</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="18"/>
+        <v>289.34205265474623</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="18"/>
+        <v>312.93938825974197</v>
+      </c>
+      <c r="K8" s="41">
+        <f t="shared" si="18"/>
+        <v>338.4612081992679</v>
+      </c>
+      <c r="L8" s="5">
+        <f>L7*(1-$Z$2)</f>
+        <v>224.3275062836185</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" ref="M8:P8" si="19">M7*(1-$Z$2)</f>
+        <v>238.75728571548521</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="19"/>
+        <v>254.11525508670408</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" si="19"/>
+        <v>270.46111985345146</v>
+      </c>
+      <c r="P8" s="41">
+        <f t="shared" si="19"/>
+        <v>287.85842600210935</v>
+      </c>
+      <c r="W8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" s="7">
+        <f>X9*'[1]Income Statement'!$H$25</f>
+        <v>31518.479999999996</v>
+      </c>
+      <c r="Y8" s="7">
+        <f>Y9*'[1]Income Statement'!$H$25</f>
+        <v>31518.479999999996</v>
+      </c>
+      <c r="Z8" s="7">
+        <f>Z9*'[1]Income Statement'!$H$25</f>
+        <v>31518.479999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="40"/>
+      <c r="W9" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="X9" s="2">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>35.979999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="40"/>
+      <c r="W10" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="40"/>
+      <c r="W11" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="X11" s="8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="Z11" s="8">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="40"/>
+      <c r="W12" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="X12" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="Z12" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="40"/>
+      <c r="W13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="X13" s="31">
+        <f>X8/'[1]Income Statement'!$F$41</f>
+        <v>22.922530909090906</v>
+      </c>
+      <c r="Y13" s="31">
+        <f>Y8/'[1]Income Statement'!$F$41</f>
+        <v>22.922530909090906</v>
+      </c>
+      <c r="Z13" s="31">
+        <f>Z8/'[1]Income Statement'!$F$41</f>
+        <v>22.922530909090906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="40"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="40"/>
+      <c r="W15" s="51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="40"/>
+      <c r="W16" s="51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="40"/>
+      <c r="W17" s="51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="40"/>
+      <c r="W18" s="51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="40"/>
+      <c r="W19" s="51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="40"/>
+      <c r="W20" s="51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="40"/>
+      <c r="W21" s="51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="40"/>
+      <c r="W22" s="51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="40"/>
+      <c r="W23" s="51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="40"/>
+      <c r="W24" s="51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="40"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B6:F6 G6:P6" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAC3436-3D57-4757-9CB9-CA7911356AEE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rNPV pipeline + self insert
</commit_message>
<xml_diff>
--- a/models/DCF_SN.xlsx
+++ b/models/DCF_SN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1785" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85C8ACB2-AF82-42FA-8EB3-09D4F844166C}"/>
+  <xr:revisionPtr revIDLastSave="1929" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27701557-E3AD-46C5-8D1E-5FD29D8782C9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="2" r:id="rId1"/>
@@ -40,8 +40,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Xavier Davis</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{9B8EEDB9-D323-4045-B792-81FFBC96CAE3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+expected ebit margin
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{3003FE48-E7A5-4F44-8CCF-C960D9B03C62}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Xavier Davis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+impact of growth eg 6% means a £1 increase in revenue increases NWC by 6pence</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
   <si>
     <t>FY</t>
   </si>
@@ -245,6 +304,102 @@
   </si>
   <si>
     <t>Share Price</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Sports Med</t>
+  </si>
+  <si>
+    <t>Launch_Central</t>
+  </si>
+  <si>
+    <t>Success_Bear</t>
+  </si>
+  <si>
+    <t>Success_Central</t>
+  </si>
+  <si>
+    <t>Success_Bull</t>
+  </si>
+  <si>
+    <t>PriceErosion</t>
+  </si>
+  <si>
+    <t>EBITMargin</t>
+  </si>
+  <si>
+    <t>WACC:</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Launch Year</t>
+  </si>
+  <si>
+    <t>Peak Sales</t>
+  </si>
+  <si>
+    <t>Adoption Speed</t>
+  </si>
+  <si>
+    <t>How to:</t>
+  </si>
+  <si>
+    <t>timeline each product between 2025 and 2029</t>
+  </si>
+  <si>
+    <t>adjust by probability</t>
+  </si>
+  <si>
+    <t>costs, commerical modelling, profit shares etc to get eah ones NPV</t>
+  </si>
+  <si>
+    <t>discount to get rNPV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum rNPVs for base portfolio or sum for segmental </t>
+  </si>
+  <si>
+    <t>adjust for overlap + correlations</t>
+  </si>
+  <si>
+    <t>equity bridge</t>
+  </si>
+  <si>
+    <t>scenario model</t>
+  </si>
+  <si>
+    <t>bridge into the SOTP as a separate operating asset</t>
+  </si>
+  <si>
+    <t>AGILI-C Cartilage Implant (CPT I adoption)</t>
+  </si>
+  <si>
+    <t>REGENETEN – Extra-articular Ligaments (broad uptake)</t>
+  </si>
+  <si>
+    <t>CORIOGRAPH Pre-Op Planning (Shoulder) – enterprise rollout</t>
+  </si>
+  <si>
+    <t>LEGION TKS Medial-Stabilised Insert – global mix-shift</t>
+  </si>
+  <si>
+    <t>CENTRIO PRP System – coverage &amp; site-of-care expansion</t>
+  </si>
+  <si>
+    <t>ALLEVYN COMPLETE CARE 5-Layer Foam – prevention protocols</t>
+  </si>
+  <si>
+    <t>Maintainance Capex</t>
+  </si>
+  <si>
+    <t>NWC pct of Sales change</t>
   </si>
 </sst>
 </file>
@@ -255,7 +410,7 @@
     <numFmt numFmtId="164" formatCode="0;\(0\);\-"/>
     <numFmt numFmtId="165" formatCode="[Color10]0.00%;[Red]\(0.00\)%;\-"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +531,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -539,7 +707,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
@@ -618,34 +786,12 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -653,7 +799,7 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -661,20 +807,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -683,6 +819,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -1920,7 +2060,7 @@
       </c>
       <c r="C28" s="27"/>
       <c r="D28" s="27">
-        <f t="shared" ref="C28:D28" si="1">D27*2</f>
+        <f t="shared" ref="D28" si="1">D27*2</f>
         <v>35.795197659661483</v>
       </c>
       <c r="G28" s="26">
@@ -2163,61 +2303,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1EAA58-ADB1-46F6-8416-C90E04EF858D}">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N28" sqref="N28"/>
+      <selection pane="topRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="54" customWidth="1"/>
-    <col min="3" max="21" width="8.88671875" style="54"/>
-    <col min="22" max="22" width="37.88671875" style="54" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.77734375" style="54" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="8.88671875" style="54"/>
-    <col min="27" max="27" width="6.88671875" style="54" hidden="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="54"/>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="22" max="22" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="34" t="s">
         <v>51</v>
       </c>
+      <c r="C1" s="34"/>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="35"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34" t="s">
+      <c r="H1" s="34" t="s">
         <v>52</v>
       </c>
+      <c r="I1" s="34"/>
       <c r="J1" s="34"/>
       <c r="K1" s="34"/>
       <c r="L1" s="34"/>
       <c r="M1" s="35"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34" t="s">
+      <c r="N1" s="34" t="s">
         <v>53</v>
       </c>
+      <c r="O1" s="34"/>
       <c r="P1" s="34"/>
       <c r="Q1" s="34"/>
       <c r="R1" s="34"/>
       <c r="S1" s="35"/>
-      <c r="T1" s="72" t="s">
+      <c r="T1" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-    </row>
-    <row r="2" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
@@ -2275,10 +2412,10 @@
       <c r="S2" s="38">
         <v>2029</v>
       </c>
-      <c r="T2" s="71">
+      <c r="T2" s="57">
         <v>2024</v>
       </c>
-      <c r="U2" s="60"/>
+      <c r="U2" s="52"/>
       <c r="V2" s="33" t="s">
         <v>1</v>
       </c>
@@ -2286,17 +2423,17 @@
         <f>'[1]Balance Sheet'!$N$7</f>
         <v>0.10567499999999999</v>
       </c>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
       <c r="AA2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="61">
+      <c r="B3" s="53">
         <f>'[1]Income Statement'!$F$43</f>
         <v>2305</v>
       </c>
@@ -2320,7 +2457,7 @@
         <f>'[1]Income Statement'!K43</f>
         <v>2902.230826911697</v>
       </c>
-      <c r="H3" s="57">
+      <c r="H3" s="45">
         <f>'[1]Income Statement'!$F$44</f>
         <v>1824</v>
       </c>
@@ -2344,7 +2481,7 @@
         <f>'[1]Income Statement'!K44</f>
         <v>2699.405880996329</v>
       </c>
-      <c r="N3" s="57">
+      <c r="N3" s="45">
         <f>'[1]Income Statement'!$F$45</f>
         <v>1681</v>
       </c>
@@ -2368,28 +2505,28 @@
         <f>'[1]Income Statement'!K45</f>
         <v>2295.8221185186958</v>
       </c>
-      <c r="T3" s="73">
+      <c r="T3" s="59">
         <f>'[1]Income Statement'!F2</f>
         <v>5810</v>
       </c>
-      <c r="U3" s="60"/>
+      <c r="U3" s="52"/>
       <c r="V3" s="33" t="s">
         <v>16</v>
       </c>
       <c r="W3" s="8">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
       <c r="AA3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="70">
+      <c r="B4" s="56">
         <v>265</v>
       </c>
       <c r="C4" s="5">
@@ -2412,7 +2549,7 @@
         <f t="shared" si="0"/>
         <v>333.66211242151832</v>
       </c>
-      <c r="H4" s="70">
+      <c r="H4" s="56">
         <v>437</v>
       </c>
       <c r="I4" s="5">
@@ -2435,7 +2572,7 @@
         <f t="shared" si="1"/>
         <v>646.73265898870386</v>
       </c>
-      <c r="N4" s="70">
+      <c r="N4" s="56">
         <v>399</v>
       </c>
       <c r="O4" s="5">
@@ -2458,11 +2595,11 @@
         <f t="shared" si="2"/>
         <v>544.93338803626386</v>
       </c>
-      <c r="T4" s="74">
+      <c r="T4" s="60">
         <f>'[1]Income Statement'!F8</f>
         <v>886</v>
       </c>
-      <c r="U4" s="60"/>
+      <c r="U4" s="52"/>
       <c r="V4" s="33" t="s">
         <v>2</v>
       </c>
@@ -2470,14 +2607,14 @@
         <f>(((W8/(W8+W6))*W7)+((W6/(W8+W6))*W5))*(1-W2)</f>
         <v>5.7975388146743925E-2</v>
       </c>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="AA4" s="64" t="s">
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="AA4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+    <row r="5" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="10">
@@ -2507,8 +2644,8 @@
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="40"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
       <c r="V5" s="33" t="s">
         <v>9</v>
       </c>
@@ -2516,87 +2653,87 @@
         <f>0.056</f>
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-    </row>
-    <row r="6" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X5" s="52"/>
+      <c r="Y5" s="52"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="5">
-        <f>B4*(1-$W$2)</f>
+        <f t="shared" ref="B6:S6" si="3">B4*(1-$W$2)</f>
         <v>236.99612500000001</v>
       </c>
       <c r="C6" s="5">
-        <f>C4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>248.17238211772872</v>
       </c>
       <c r="D6" s="5">
-        <f>D4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>259.87568887882856</v>
       </c>
       <c r="E6" s="5">
-        <f>E4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>272.13089987671583</v>
       </c>
       <c r="F6" s="5">
-        <f>F4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>284.96404179707872</v>
       </c>
       <c r="G6" s="40">
-        <f>G4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>298.40236869137436</v>
       </c>
       <c r="H6" s="5">
-        <f>H4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>390.82002500000004</v>
       </c>
       <c r="I6" s="5">
-        <f>I4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>422.69341224690044</v>
       </c>
       <c r="J6" s="5">
-        <f>J4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>457.16623849284122</v>
       </c>
       <c r="K6" s="5">
-        <f>K4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>494.45050138518189</v>
       </c>
       <c r="L6" s="5">
-        <f>L4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>534.77548807201822</v>
       </c>
       <c r="M6" s="40">
-        <f>M4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>578.38918525007261</v>
       </c>
       <c r="N6" s="5">
-        <f>N4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>356.83567500000004</v>
       </c>
       <c r="O6" s="5">
-        <f>O4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>379.7889907523774</v>
       </c>
       <c r="P6" s="5">
-        <f>P4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>404.21876959670419</v>
       </c>
       <c r="Q6" s="5">
-        <f>Q4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>430.21998444606209</v>
       </c>
       <c r="R6" s="5">
-        <f>R4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>457.89371730916037</v>
       </c>
       <c r="S6" s="40">
-        <f>S4*(1-$W$2)</f>
+        <f t="shared" si="3"/>
         <v>487.3475522555317</v>
       </c>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
       <c r="V6" s="33" t="s">
         <v>10</v>
       </c>
@@ -2604,30 +2741,30 @@
         <f>'[1]Balance Sheet'!$F$49</f>
         <v>2986</v>
       </c>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-    </row>
-    <row r="7" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
-      <c r="B7" s="53"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="40"/>
-      <c r="H7" s="59"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="40"/>
-      <c r="N7" s="59"/>
+      <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="40"/>
-      <c r="T7" s="59"/>
+      <c r="T7" s="5"/>
       <c r="V7" s="33" t="s">
         <v>11</v>
       </c>
@@ -2636,81 +2773,81 @@
         <v>6.6460000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A8" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="63">
+      <c r="B8" s="28">
         <v>213</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="54">
         <f>$B$9*'[1]Income Statement'!G39</f>
         <v>224.90961461788868</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="54">
         <f>$B$9*'[1]Income Statement'!H39</f>
         <v>239.10575461472399</v>
       </c>
-      <c r="E8" s="68">
+      <c r="E8" s="54">
         <f>$B$9*'[1]Income Statement'!I39</f>
         <v>254.24485396145781</v>
       </c>
-      <c r="F8" s="68">
+      <c r="F8" s="54">
         <f>$B$9*'[1]Income Statement'!J39</f>
         <v>270.39244614722719</v>
       </c>
-      <c r="G8" s="69">
+      <c r="G8" s="55">
         <f>$B$9*'[1]Income Statement'!K39</f>
         <v>287.61879333642975</v>
       </c>
-      <c r="H8" s="67">
+      <c r="H8" s="1">
         <v>98</v>
       </c>
-      <c r="I8" s="65">
+      <c r="I8" s="1">
         <f>$H$9*'[1]Income Statement'!G39</f>
         <v>103.47954099790184</v>
       </c>
-      <c r="J8" s="65">
+      <c r="J8" s="1">
         <f>$H$9*'[1]Income Statement'!H39</f>
         <v>110.01109836733779</v>
       </c>
-      <c r="K8" s="65">
+      <c r="K8" s="1">
         <f>$H$9*'[1]Income Statement'!I39</f>
         <v>116.97650557851111</v>
       </c>
-      <c r="L8" s="65">
+      <c r="L8" s="1">
         <f>$H$9*'[1]Income Statement'!J39</f>
         <v>124.40591418980407</v>
       </c>
-      <c r="M8" s="66">
+      <c r="M8" s="39">
         <f>$H$9*'[1]Income Statement'!K39</f>
         <v>132.33165139422587</v>
       </c>
-      <c r="N8" s="67">
+      <c r="N8" s="1">
         <v>62</v>
       </c>
-      <c r="O8" s="65">
+      <c r="O8" s="1">
         <f>$N$9*'[1]Income Statement'!G39</f>
         <v>65.466648386427678</v>
       </c>
-      <c r="P8" s="65">
+      <c r="P8" s="1">
         <f>$N$9*'[1]Income Statement'!H39</f>
         <v>69.598858150764727</v>
       </c>
-      <c r="Q8" s="65">
+      <c r="Q8" s="1">
         <f>$N$9*'[1]Income Statement'!I39</f>
         <v>74.00554434558866</v>
       </c>
-      <c r="R8" s="65">
+      <c r="R8" s="1">
         <f>$N$9*'[1]Income Statement'!J39</f>
         <v>78.705782446610726</v>
       </c>
-      <c r="S8" s="66">
+      <c r="S8" s="39">
         <f>$N$9*'[1]Income Statement'!K39</f>
         <v>83.720024351449027</v>
       </c>
-      <c r="T8" s="67"/>
-      <c r="U8" s="67"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
       <c r="V8" s="33" t="s">
         <v>12</v>
       </c>
@@ -2718,11 +2855,11 @@
         <f>W9*('[1]Income Statement'!$F$25*'[1]Income Statement'!$N$8)</f>
         <v>16127.16</v>
       </c>
-      <c r="X8" s="67"/>
-      <c r="Y8" s="67"/>
-    </row>
-    <row r="9" spans="1:28" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62" t="s">
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A9" s="43" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="10">
@@ -2730,29 +2867,29 @@
         <v>0.47438752783964366</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="10">
         <f>H8/'[1]Income Statement'!F39</f>
         <v>0.21826280623608019</v>
       </c>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="66"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="39"/>
       <c r="N9" s="10">
         <f>N8/'[1]Income Statement'!F39</f>
         <v>0.13808463251670378</v>
       </c>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="67"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="1"/>
       <c r="V9" s="33" t="s">
         <v>13</v>
       </c>
@@ -2760,27 +2897,27 @@
         <v>36.82</v>
       </c>
     </row>
-    <row r="10" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="44"/>
-      <c r="B10" s="53"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="40"/>
-      <c r="H10" s="59"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="40"/>
-      <c r="N10" s="59"/>
+      <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
       <c r="S10" s="40"/>
-      <c r="T10" s="59"/>
+      <c r="T10" s="5"/>
       <c r="V10" s="33" t="s">
         <v>14</v>
       </c>
@@ -2788,8 +2925,8 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="11" spans="1:28" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A11" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1">
@@ -2864,7 +3001,7 @@
         <f>'[1]Balance Sheet'!K53*$N$13</f>
         <v>-166.24353726809963</v>
       </c>
-      <c r="T11" s="67"/>
+      <c r="T11" s="1"/>
       <c r="V11" s="33" t="s">
         <v>15</v>
       </c>
@@ -2872,8 +3009,8 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62" t="s">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A12" s="43" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1">
@@ -2948,7 +3085,7 @@
         <f>DCF!F6*$N$13</f>
         <v>-40.661494861959234</v>
       </c>
-      <c r="T12" s="67"/>
+      <c r="T12" s="1"/>
       <c r="V12" s="33" t="s">
         <v>17</v>
       </c>
@@ -2956,38 +3093,38 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A13" s="43" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="10">
         <f>(B3-B4)/((B3-B4)+(H3-H4)+(N3-N4))</f>
         <v>0.43321299638989169</v>
       </c>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="39"/>
       <c r="H13" s="10">
         <f>(H3-H4)/((B3-B4)+(H3-H4)+(N3-N4))</f>
         <v>0.29454236568273517</v>
       </c>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="65"/>
-      <c r="L13" s="65"/>
-      <c r="M13" s="66"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="39"/>
       <c r="N13" s="10">
         <f>(N3-N4)/((B3-B4)+(H3-H4)+(N3-N4))</f>
         <v>0.27224463792737313</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="65"/>
-      <c r="S13" s="66"/>
-      <c r="T13" s="67"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="1"/>
       <c r="V13" s="33" t="s">
         <v>49</v>
       </c>
@@ -2996,200 +3133,193 @@
         <v>12.080269662921348</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A14" s="43"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="66"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="39"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="66"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="39"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="65"/>
-      <c r="R14" s="65"/>
-      <c r="S14" s="66"/>
-      <c r="T14" s="67"/>
-      <c r="U14"/>
-      <c r="AA14"/>
-      <c r="AB14"/>
-    </row>
-    <row r="15" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5">
-        <f t="shared" ref="C15:S15" si="3">SUM(C12,C11,C8,C6)</f>
+        <f t="shared" ref="C15:S15" si="4">SUM(C12,C11,C8,C6)</f>
         <v>201.51828811100489</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>214.36083940975044</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>227.83096771892707</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>241.95995880658955</v>
       </c>
       <c r="G15" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>256.78070528418471</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>341.53625527306815</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>373.66323006398613</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>408.44582149928374</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>446.10248759809065</v>
       </c>
       <c r="M15" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>486.86960453478866</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>274.59648499333781</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>294.9531108673541</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>316.61061908337911</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>339.65128879765717</v>
       </c>
       <c r="S15" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>364.16254447692188</v>
       </c>
-      <c r="T15" s="59"/>
+      <c r="T15" s="5"/>
       <c r="U15"/>
-      <c r="V15" s="64"/>
+      <c r="V15"/>
       <c r="AA15"/>
     </row>
-    <row r="16" spans="1:28" s="64" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="75" t="s">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A16" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76">
+      <c r="B16" s="62"/>
+      <c r="C16" s="62">
         <f>C15/((1+$W$4)^(C2-2024))</f>
         <v>190.47540270667787</v>
       </c>
-      <c r="D16" s="76">
+      <c r="D16" s="62">
         <f>D15/((1+$W$4)^(D2-2024))</f>
         <v>191.51126259893149</v>
       </c>
-      <c r="E16" s="76">
+      <c r="E16" s="62">
         <f>E15/((1+$W$4)^(E2-2024))</f>
         <v>192.39157969931165</v>
       </c>
-      <c r="F16" s="76">
+      <c r="F16" s="62">
         <f>F15/((1+$W$4)^(F2-2024))</f>
         <v>193.12622116425743</v>
       </c>
-      <c r="G16" s="77">
+      <c r="G16" s="63">
         <f>G15/((1+$W$4)^(G2-2024))</f>
         <v>193.72450666737925</v>
       </c>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76">
+      <c r="H16" s="62"/>
+      <c r="I16" s="62">
         <f>I15/((1+$W$4)^(I2-2024))</f>
         <v>322.82060537470289</v>
       </c>
-      <c r="J16" s="76">
+      <c r="J16" s="62">
         <f>J15/((1+$W$4)^(J2-2024))</f>
         <v>333.83297608552834</v>
       </c>
-      <c r="K16" s="76">
+      <c r="K16" s="62">
         <f>K15/((1+$W$4)^(K2-2024))</f>
         <v>344.91157021628231</v>
       </c>
-      <c r="L16" s="76">
+      <c r="L16" s="62">
         <f>L15/((1+$W$4)^(L2-2024))</f>
         <v>356.06754153343797</v>
       </c>
-      <c r="M16" s="77">
+      <c r="M16" s="63">
         <f>M15/((1+$W$4)^(M2-2024))</f>
         <v>367.3117645091736</v>
       </c>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76">
+      <c r="N16" s="62"/>
+      <c r="O16" s="62">
         <f>O15/((1+$W$4)^(O2-2024))</f>
         <v>259.54902927784417</v>
       </c>
-      <c r="P16" s="76">
+      <c r="P16" s="62">
         <f>P15/((1+$W$4)^(P2-2024))</f>
         <v>263.51288241466108</v>
       </c>
-      <c r="Q16" s="76">
+      <c r="Q16" s="62">
         <f>Q15/((1+$W$4)^(Q2-2024))</f>
         <v>267.36144679934995</v>
       </c>
-      <c r="R16" s="76">
+      <c r="R16" s="62">
         <f>R15/((1+$W$4)^(R2-2024))</f>
         <v>271.10093026381759</v>
       </c>
-      <c r="S16" s="77">
+      <c r="S16" s="63">
         <f>S15/((1+$W$4)^(S2-2024))</f>
         <v>274.73718945297367</v>
       </c>
-      <c r="T16" s="67"/>
-      <c r="U16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-    </row>
-    <row r="17" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="36"/>
-      <c r="B17" s="55"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="58"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="39"/>
-      <c r="N17" s="58"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="39"/>
-      <c r="T17" s="58"/>
-      <c r="V17" s="64"/>
-    </row>
-    <row r="18" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="5">
@@ -3219,14 +3349,13 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="39"/>
-      <c r="T18" s="58"/>
-      <c r="V18" s="64"/>
-    </row>
-    <row r="19" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="78">
+      <c r="B19" s="64">
         <f>B18+SUM(C16:G16)</f>
         <v>4886.8167262570896</v>
       </c>
@@ -3235,7 +3364,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="39"/>
-      <c r="H19" s="78">
+      <c r="H19" s="64">
         <f>H18+SUM(I16:M16)</f>
         <v>9168.0634995460532</v>
       </c>
@@ -3244,7 +3373,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="39"/>
-      <c r="N19" s="78">
+      <c r="N19" s="64">
         <f>N18+SUM(O16:S16)</f>
         <v>6903.4711455820134</v>
       </c>
@@ -3253,10 +3382,9 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="39"/>
-      <c r="T19" s="58"/>
-      <c r="V19" s="64"/>
-    </row>
-    <row r="20" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="28"/>
       <c r="C20" s="1"/>
@@ -3264,43 +3392,41 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="39"/>
-      <c r="H20" s="58"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="39"/>
-      <c r="N20" s="58"/>
+      <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="39"/>
-      <c r="T20" s="58"/>
-    </row>
-    <row r="21" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="39"/>
-      <c r="H21" s="58"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="39"/>
-      <c r="N21" s="58"/>
+      <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="39"/>
-      <c r="T21" s="58"/>
-    </row>
-    <row r="22" spans="1:22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="26">
         <f>B19</f>
@@ -3371,16 +3497,16 @@
         <f>R22+0.005</f>
         <v>6.7975388146743934E-2</v>
       </c>
-      <c r="T22" s="58"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
       <c r="B23" s="25">
         <f>B24-0.005</f>
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="C23" s="13">
-        <f t="dataTable" ref="C23:G27" dt2D="1" dtr="1" r1="W4" r2="W12" ca="1"/>
+        <f t="dataTable" ref="C23:G27" dt2D="1" dtr="1" r1="W4" r2="W12"/>
         <v>5263.5337170491621</v>
       </c>
       <c r="D23" s="13">
@@ -3400,7 +3526,7 @@
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="I23" s="13">
-        <f t="dataTable" ref="I23:M27" dt2D="1" dtr="1" r1="W4" r2="W12"/>
+        <f t="dataTable" ref="I23:M27" dt2D="1" dtr="1" r1="W4" r2="W12" ca="1"/>
         <v>9880.4455126833091</v>
       </c>
       <c r="J23" s="13">
@@ -3435,9 +3561,9 @@
       <c r="S23" s="15">
         <v>4585.5468610883636</v>
       </c>
-      <c r="T23" s="58"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T23" s="1"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B24" s="25">
         <f>B25-0.005</f>
         <v>1.4999999999999999E-2</v>
@@ -3495,9 +3621,9 @@
       <c r="S24" s="15">
         <v>4913.563797236091</v>
       </c>
-      <c r="T24" s="58"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B25" s="25">
         <v>0.02</v>
       </c>
@@ -3552,9 +3678,9 @@
       <c r="S25" s="15">
         <v>5309.9526525738038</v>
       </c>
-      <c r="T25" s="58"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B26" s="25">
         <f>B25+0.005</f>
         <v>2.5000000000000001E-2</v>
@@ -3612,9 +3738,9 @@
       <c r="S26" s="15">
         <v>5798.5777557806932</v>
       </c>
-      <c r="T26" s="58"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B27" s="25">
         <f>B26+0.005</f>
         <v>3.0000000000000002E-2</v>
@@ -3672,93 +3798,89 @@
       <c r="S27" s="16">
         <v>6415.8717487745016</v>
       </c>
-      <c r="T27" s="58"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="83" t="s">
+      <c r="B28" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
-      <c r="H28" s="83" t="s">
+      <c r="H28" s="66" t="s">
         <v>38</v>
       </c>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="84"/>
+      <c r="K28" s="30"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
-      <c r="N28" s="83" t="s">
+      <c r="N28" s="66" t="s">
         <v>38</v>
       </c>
       <c r="O28" s="30"/>
       <c r="P28" s="30"/>
-      <c r="Q28" s="84"/>
+      <c r="Q28" s="30"/>
       <c r="R28" s="30"/>
       <c r="S28" s="30"/>
-      <c r="T28" s="58"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="85">
+      <c r="B29" s="67">
         <f>IF(B28="Bull",D26,IF(B28="Bear",F24,IF(B28="Central",E25,"Error")))</f>
         <v>4886.8167262570896</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="85">
+      <c r="G29" s="68"/>
+      <c r="H29" s="67">
         <f>IF(H28="Bull",J26,IF(H28="Bear",L24,IF(H28="Central",K25,"Error")))</f>
         <v>9168.0634995460532</v>
       </c>
       <c r="I29" s="30"/>
-      <c r="J29" s="84"/>
+      <c r="J29" s="30"/>
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
-      <c r="M29" s="86"/>
-      <c r="N29" s="85">
+      <c r="M29" s="68"/>
+      <c r="N29" s="67">
         <f>IF(N28="Bull",P26,IF(N28="Bear",R24,IF(N28="Central",Q25,"Error")))</f>
         <v>6903.4711455820134</v>
       </c>
       <c r="O29" s="30"/>
-      <c r="P29" s="84"/>
+      <c r="P29" s="30"/>
       <c r="Q29" s="30"/>
       <c r="R29" s="30"/>
-      <c r="S29" s="86"/>
-      <c r="T29" s="58"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="B30"/>
-      <c r="C30"/>
+      <c r="S29" s="68"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D30" s="28"/>
       <c r="E30" s="27"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>25</v>
       </c>
@@ -3766,121 +3888,120 @@
         <f>DCF!B25</f>
         <v>2986</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="28"/>
       <c r="E31" s="27"/>
       <c r="F31" s="10"/>
-      <c r="G31"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
-      <c r="T31" s="58"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="52" t="s">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="79">
+      <c r="B32" s="64">
         <f>B29+H29+N29</f>
         <v>20958.351371385157</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
-      <c r="T32" s="58"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="80">
+      <c r="B33" s="65">
         <f>B32/DCF!B36</f>
         <v>23.925058643133742</v>
       </c>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
-      <c r="T33" s="58"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="56">
+      <c r="B34" s="3">
         <f>B33*2</f>
         <v>47.850117286267484</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="54">
+      <c r="B35">
         <f>DCF!I9</f>
         <v>36.82</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="82">
+      <c r="B36" s="27">
         <f>B34-B35</f>
         <v>11.030117286267483</v>
       </c>
@@ -3890,7 +4011,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28 H28 N28" xr:uid="{B110F3C2-1E4E-45A0-BB92-5A75057DEE2A}">
       <formula1>$AA$2:$AA$4</formula1>
     </dataValidation>
@@ -3900,13 +4021,383 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAC3436-3D57-4757-9CB9-CA7911356AEE}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAC3436-3D57-4757-9CB9-CA7911356AEE}">
+  <dimension ref="B2:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>2027</v>
+      </c>
+      <c r="E3">
+        <v>0.45</v>
+      </c>
+      <c r="F3">
+        <v>0.65</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+      <c r="H3" s="70">
+        <v>0.02</v>
+      </c>
+      <c r="I3" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="J3" s="69">
+        <v>0.02</v>
+      </c>
+      <c r="K3" s="69">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>2028</v>
+      </c>
+      <c r="E4">
+        <v>0.35</v>
+      </c>
+      <c r="F4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G4">
+        <v>0.75</v>
+      </c>
+      <c r="H4" s="70">
+        <v>0.03</v>
+      </c>
+      <c r="I4" s="69">
+        <v>0.26</v>
+      </c>
+      <c r="J4" s="69">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K4" s="69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>2027</v>
+      </c>
+      <c r="E5">
+        <v>0.45</v>
+      </c>
+      <c r="F5">
+        <v>0.65</v>
+      </c>
+      <c r="G5">
+        <v>0.8</v>
+      </c>
+      <c r="H5" s="70">
+        <v>0.02</v>
+      </c>
+      <c r="I5" s="69">
+        <v>0.2</v>
+      </c>
+      <c r="J5" s="69">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K5" s="69">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>2027</v>
+      </c>
+      <c r="E6">
+        <v>0.5</v>
+      </c>
+      <c r="F6">
+        <v>0.7</v>
+      </c>
+      <c r="G6">
+        <v>0.85</v>
+      </c>
+      <c r="H6" s="70">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="69">
+        <v>0.16</v>
+      </c>
+      <c r="J6" s="69">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K6" s="69">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7">
+        <v>2027</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G7">
+        <v>0.75</v>
+      </c>
+      <c r="H7" s="70">
+        <v>0.01</v>
+      </c>
+      <c r="I7" s="69">
+        <v>0.24</v>
+      </c>
+      <c r="J7" s="69">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K7" s="69">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8">
+        <v>2028</v>
+      </c>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.6</v>
+      </c>
+      <c r="G8">
+        <v>0.8</v>
+      </c>
+      <c r="H8" s="70">
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="69">
+        <v>0.23</v>
+      </c>
+      <c r="J8" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="K8" s="69">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H9" s="70"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <f>SOTP!W2</f>
+        <v>0.10567499999999999</v>
+      </c>
+      <c r="J10" s="69"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="8">
+        <f>SOTP!W4</f>
+        <v>5.7975388146743925E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="71">
+        <v>-1</v>
+      </c>
+      <c r="J14" s="71">
+        <v>0</v>
+      </c>
+      <c r="K14" s="71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H18" s="72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H19" s="72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H20" s="72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H21" s="72" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H22" s="72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H23" s="72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H24" s="72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H25" s="72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H26" s="72" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H27" s="72" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comps analysis + net debt sign issues
</commit_message>
<xml_diff>
--- a/models/DCF_SN.xlsx
+++ b/models/DCF_SN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4230" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77FF4F57-071C-42C2-843C-D8958B9DFD93}"/>
+  <xr:revisionPtr revIDLastSave="4235" documentId="8_{4CAA811A-3924-48A6-9DA9-F0A76AB10370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{519D48C8-EC6A-4AA6-B0C7-A4444671E752}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{074DC5BB-03BC-4711-88CA-6F8F6CA366FE}"/>
   </bookViews>
@@ -1678,9 +1678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C2E0D3-EC22-43DB-ABCF-85A4F712E8DB}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D27" sqref="D27"/>
+      <selection pane="topRight" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2095,7 +2095,7 @@
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="H17" s="13">
-        <f t="dataTable" ref="H17:L21" dt2D="1" dtr="1" r1="I4" r2="I12"/>
+        <f t="dataTable" ref="H17:L21" dt2D="1" dtr="1" r1="I4" r2="I12" ca="1"/>
         <v>20738.04588044636</v>
       </c>
       <c r="I17" s="13">
@@ -2257,7 +2257,7 @@
       </c>
       <c r="L23" s="27">
         <f>I23-B25</f>
-        <v>22984.559034191887</v>
+        <v>17012.559034191887</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="J24" s="83">
         <f>L23/B36*2</f>
-        <v>52.476162178520291</v>
+        <v>38.841458982173258</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -2281,19 +2281,19 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f>-(SUM(B15:B22)+(-1*SUM(B23:B24)))</f>
-        <v>-2986</v>
+        <f>(SUM(B15:B22)+(-1*SUM(B23:B24)))</f>
+        <v>2986</v>
       </c>
       <c r="I25" s="28" t="s">
         <v>43</v>
       </c>
       <c r="J25" s="83">
         <f>J24-B29</f>
-        <v>15.65616217852029</v>
+        <v>2.0214589821732574</v>
       </c>
       <c r="K25" s="10">
         <f>J25/B29</f>
-        <v>0.42520809827594486</v>
+        <v>5.4901113041098785E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2301,11 +2301,11 @@
         <v>19</v>
       </c>
       <c r="B26" s="5">
-        <f>B12+B25</f>
+        <f>B12-B25</f>
         <v>17012.559034191887</v>
       </c>
       <c r="D26" s="5">
-        <f>D12+B25</f>
+        <f>D12-B25</f>
         <v>15678.29657493173</v>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
         <v>10.08</v>
       </c>
       <c r="H29" s="13">
-        <f t="dataTable" ref="H29:L33" dt2D="1" dtr="1" r1="I4" r2="I13" ca="1"/>
+        <f t="dataTable" ref="H29:L33" dt2D="1" dtr="1" r1="I4" r2="I13"/>
         <v>16801.597649603467</v>
       </c>
       <c r="I29" s="13">
@@ -2588,7 +2588,7 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A21" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C36" sqref="C36"/>
+      <selection pane="topRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3784,7 +3784,7 @@
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="C23" s="13">
-        <f t="dataTable" ref="C23:G27" dt2D="1" dtr="1" r1="W4" r2="W12" ca="1"/>
+        <f t="dataTable" ref="C23:G27" dt2D="1" dtr="1" r1="W4" r2="W12"/>
         <v>5263.5337170491621</v>
       </c>
       <c r="D23" s="13">
@@ -3824,7 +3824,7 @@
         <v>9.9999999999999985E-3</v>
       </c>
       <c r="O23" s="13">
-        <f t="dataTable" ref="O23:S27" dt2D="1" dtr="1" r1="W4" r2="W12"/>
+        <f t="dataTable" ref="O23:S27" dt2D="1" dtr="1" r1="W4" r2="W12" ca="1"/>
         <v>7437.2030569098843</v>
       </c>
       <c r="P23" s="13">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="B31" s="1">
         <f>DCF!B25</f>
-        <v>-2986</v>
+        <v>2986</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="28"/>
@@ -4189,7 +4189,7 @@
         <v>64</v>
       </c>
       <c r="B32" s="63">
-        <f>B29+H29+N29+B31</f>
+        <f>B29+H29+N29-B31</f>
         <v>17972.351371385157</v>
       </c>
       <c r="C32" s="1"/>
@@ -4317,10 +4317,10 @@
   <dimension ref="A1:BL57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q51" sqref="Q51"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="B52" s="113">
         <f>SOTP!B31</f>
-        <v>-2986</v>
+        <v>2986</v>
       </c>
       <c r="C52" s="71"/>
       <c r="D52" s="71"/>
@@ -10893,7 +10893,7 @@
         <v>64</v>
       </c>
       <c r="B53" s="113">
-        <f>E50+K50+Q50+B52</f>
+        <f>E50+K50+Q50-B52</f>
         <v>22498.871460405269</v>
       </c>
       <c r="C53" s="71"/>

</xml_diff>